<commit_message>
fix: false count result
</commit_message>
<xml_diff>
--- a/assets/temp/file-lulus.xlsx
+++ b/assets/temp/file-lulus.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858DD58D-0F41-4EA9-B5BB-96656971C09A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D1C4D2-24B2-4C42-9792-73D1CA5694DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E69066C1-6376-4D70-91CF-8BA6857E787E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>NISN Siswa</t>
   </si>
@@ -84,6 +84,36 @@
   </si>
   <si>
     <t>Akutuh</t>
+  </si>
+  <si>
+    <t>0054497273</t>
+  </si>
+  <si>
+    <t>0054497274</t>
+  </si>
+  <si>
+    <t>0054497275</t>
+  </si>
+  <si>
+    <t>0054497276</t>
+  </si>
+  <si>
+    <t>0054497277</t>
+  </si>
+  <si>
+    <t>0054497278</t>
+  </si>
+  <si>
+    <t>0054497279</t>
+  </si>
+  <si>
+    <t>0054497280</t>
+  </si>
+  <si>
+    <t>0054497281</t>
+  </si>
+  <si>
+    <t>0054497282</t>
   </si>
 </sst>
 </file>
@@ -91,9 +121,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +135,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -151,8 +187,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73F65474-EAC1-4E0C-B28E-6DB060A5068B}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A5" sqref="A5:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -523,7 +559,148 @@
         <v>16</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" s="6">
+        <v>44544</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6">
+        <v>44545</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6">
+        <v>44546</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7" s="6">
+        <v>44547</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8" s="6">
+        <v>44548</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="C9" s="6">
+        <v>44549</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10" s="6">
+        <v>44550</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>11</v>
+      </c>
+      <c r="C11" s="6">
+        <v>44551</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+      <c r="C12" s="6">
+        <v>44552</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
+      </c>
+      <c r="C13" s="6">
+        <v>44553</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>